<commit_message>
LonePair Core part Update
</commit_message>
<xml_diff>
--- a/SLAM_Ext/validation/EwaldTestValidation.xlsx
+++ b/SLAM_Ext/validation/EwaldTestValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woongkyujee/Desktop/ProjectPAX/SLAM Extension Reference/SLAM-3D-Extension/SLAM_Ext/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2504ADA7-FA6C-6A42-847B-4E07AA6494E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA4AE85-F2D3-6A47-A36E-7F8B4CA13263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17100" yWindow="1000" windowWidth="47980" windowHeight="25400" firstSheet="4" activeTab="16" xr2:uid="{ED569559-3BE8-BA43-B08A-1C36884B8A7F}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="211">
   <si>
     <t>GULP</t>
   </si>
@@ -15778,8 +15778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62A30DF-D5DC-0A4A-9B65-326D1235E053}">
   <dimension ref="C4:V68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16613,23 +16613,23 @@
         <v>131</v>
       </c>
       <c r="I27" s="19">
-        <v>-2.0471180000000002</v>
+        <v>-1.0234909999999999</v>
       </c>
       <c r="J27" s="19">
-        <v>4.5241990000000003</v>
+        <v>4.252084</v>
       </c>
       <c r="K27" s="19">
-        <v>-11.362907999999999</v>
+        <v>-11.261998999999999</v>
       </c>
       <c r="L27" s="19"/>
       <c r="M27" s="19">
-        <v>-8.8026079999999993</v>
+        <v>-4.4010119999999997</v>
       </c>
       <c r="N27" s="19">
-        <v>12.446401</v>
+        <v>13.633868</v>
       </c>
       <c r="O27" s="19">
-        <v>-35.408051</v>
+        <v>-32.93562</v>
       </c>
       <c r="Q27" t="s">
         <v>131</v>
@@ -16664,23 +16664,23 @@
         <v>131</v>
       </c>
       <c r="I28" s="19">
-        <v>11.367488</v>
+        <v>9.800065</v>
       </c>
       <c r="J28" s="19">
-        <v>5.4103960000000004</v>
+        <v>4.9997689999999997</v>
       </c>
       <c r="K28" s="19">
-        <v>-6.1022400000000001</v>
+        <v>-5.2988299999999997</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="19">
-        <v>48.880198999999998</v>
+        <v>42.140281999999999</v>
       </c>
       <c r="N28" s="19">
-        <v>44.587923000000004</v>
+        <v>39.688825999999999</v>
       </c>
       <c r="O28" s="19">
-        <v>1.0046649999999999</v>
+        <v>0.39214399999999999</v>
       </c>
       <c r="Q28" t="s">
         <v>131</v>
@@ -16706,23 +16706,23 @@
         <v>131</v>
       </c>
       <c r="I29" s="19">
-        <v>-9.4280810000000006</v>
+        <v>-8.7362950000000001</v>
       </c>
       <c r="J29" s="19">
-        <v>-1.3180750000000001</v>
+        <v>-1.9084589999999999</v>
       </c>
       <c r="K29" s="19">
-        <v>8.9899999999999995E-4</v>
+        <v>-0.40294999999999997</v>
       </c>
       <c r="L29" s="19"/>
       <c r="M29" s="19">
-        <v>-40.540748999999998</v>
+        <v>-37.566068999999999</v>
       </c>
       <c r="N29" s="19">
-        <v>-25.178766</v>
+        <v>-25.889963000000002</v>
       </c>
       <c r="O29" s="19">
-        <v>-16.214956999999998</v>
+        <v>-15.171176000000001</v>
       </c>
       <c r="Q29" t="s">
         <v>131</v>
@@ -16751,23 +16751,23 @@
         <v>205</v>
       </c>
       <c r="I30" s="19">
-        <v>0</v>
+        <v>41.471775000000001</v>
       </c>
       <c r="J30" s="19">
-        <v>0</v>
+        <v>-23.825254999999999</v>
       </c>
       <c r="K30" s="19">
-        <v>0</v>
+        <v>234.990309</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="19">
-        <v>0</v>
+        <v>178.328633</v>
       </c>
       <c r="N30" s="19">
-        <v>0</v>
+        <v>0.44123000000000001</v>
       </c>
       <c r="O30" s="19">
-        <v>0</v>
+        <v>650.40279099999998</v>
       </c>
       <c r="Q30" t="s">
         <v>131</v>
@@ -16799,23 +16799,23 @@
         <v>132</v>
       </c>
       <c r="I31" s="19">
-        <v>0.40865200000000002</v>
+        <v>-8.3417000000000005E-2</v>
       </c>
       <c r="J31" s="19">
-        <v>3.1209039999999999</v>
+        <v>3.2641990000000001</v>
       </c>
       <c r="K31" s="19">
-        <v>-2.2203349999999999</v>
+        <v>-2.0026410000000001</v>
       </c>
       <c r="L31" s="19"/>
       <c r="M31" s="19">
-        <v>1.7572030000000001</v>
+        <v>-0.35869200000000001</v>
       </c>
       <c r="N31" s="19">
-        <v>12.500563</v>
+        <v>11.976236</v>
       </c>
       <c r="O31" s="19">
-        <v>-7.9711449999999999</v>
+        <v>-8.5566589999999998</v>
       </c>
       <c r="Q31" t="s">
         <v>131</v>
@@ -16850,23 +16850,23 @@
         <v>132</v>
       </c>
       <c r="I32" s="19">
-        <v>-5.5788989999999998</v>
+        <v>-4.5879310000000002</v>
       </c>
       <c r="J32" s="19">
-        <v>-4.3061910000000001</v>
+        <v>-5.7087079999999997</v>
       </c>
       <c r="K32" s="19">
-        <v>-3.253889</v>
+        <v>-4.0926030000000004</v>
       </c>
       <c r="L32" s="19"/>
       <c r="M32" s="19">
-        <v>-23.989267000000002</v>
+        <v>-19.728103000000001</v>
       </c>
       <c r="N32" s="19">
-        <v>-28.030497</v>
+        <v>-31.122761000000001</v>
       </c>
       <c r="O32" s="19">
-        <v>-13.085846999999999</v>
+        <v>-11.553561999999999</v>
       </c>
       <c r="Q32" t="s">
         <v>131</v>
@@ -16901,23 +16901,23 @@
         <v>132</v>
       </c>
       <c r="I33" s="19">
-        <v>3.1094900000000001</v>
+        <v>-13.287725</v>
       </c>
       <c r="J33" s="19">
-        <v>4.289612</v>
+        <v>-39.886091999999998</v>
       </c>
       <c r="K33" s="19">
-        <v>-3.6471439999999999</v>
+        <v>135.25022000000001</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="19">
-        <v>13.370805000000001</v>
+        <v>-57.137216000000002</v>
       </c>
       <c r="N33" s="19">
-        <v>22.659527000000001</v>
+        <v>-177.10079400000001</v>
       </c>
       <c r="O33" s="19">
-        <v>-7.5446749999999998</v>
+        <v>334.565021</v>
       </c>
       <c r="Q33" t="s">
         <v>205</v>
@@ -16952,23 +16952,23 @@
         <v>132</v>
       </c>
       <c r="I34" s="19">
-        <v>2.6659160000000002</v>
+        <v>2.1743739999999998</v>
       </c>
       <c r="J34" s="19">
-        <v>0.35392499999999999</v>
+        <v>-0.480657</v>
       </c>
       <c r="K34" s="19">
-        <v>-3.252564</v>
+        <v>-3.2465419999999998</v>
       </c>
       <c r="L34" s="19"/>
       <c r="M34" s="19">
-        <v>11.463438</v>
+        <v>9.3498070000000002</v>
       </c>
       <c r="N34" s="19">
-        <v>7.0497050000000003</v>
+        <v>2.884979</v>
       </c>
       <c r="O34" s="19">
-        <v>-2.9361459999999999</v>
+        <v>-2.8865980000000002</v>
       </c>
       <c r="Q34" t="s">
         <v>132</v>
@@ -16994,23 +16994,23 @@
         <v>131</v>
       </c>
       <c r="I35" s="19">
-        <v>2.063202</v>
+        <v>1.984483</v>
       </c>
       <c r="J35" s="19">
-        <v>0.232404</v>
+        <v>0.30060500000000001</v>
       </c>
       <c r="K35" s="19">
-        <v>0.57449600000000001</v>
+        <v>0.46485399999999999</v>
       </c>
       <c r="L35" s="19"/>
       <c r="M35" s="19">
-        <v>8.8717699999999997</v>
+        <v>8.5332760000000007</v>
       </c>
       <c r="N35" s="19">
-        <v>5.3013380000000003</v>
+        <v>5.3860619999999999</v>
       </c>
       <c r="O35" s="19">
-        <v>4.9457069999999996</v>
+        <v>4.4649010000000002</v>
       </c>
       <c r="Q35" t="s">
         <v>132</v>
@@ -17045,23 +17045,23 @@
         <v>131</v>
       </c>
       <c r="I36" s="19">
-        <v>1.364654</v>
+        <v>1.0947519999999999</v>
       </c>
       <c r="J36" s="19">
-        <v>0.51017299999999999</v>
+        <v>0.51624199999999998</v>
       </c>
       <c r="K36" s="19">
-        <v>-0.70043699999999998</v>
+        <v>-0.52163400000000004</v>
       </c>
       <c r="L36" s="19"/>
       <c r="M36" s="19">
-        <v>5.8680099999999999</v>
+        <v>4.7074319999999998</v>
       </c>
       <c r="N36" s="19">
-        <v>4.8338429999999999</v>
+        <v>4.2761529999999999</v>
       </c>
       <c r="O36" s="19">
-        <v>0.35542299999999999</v>
+        <v>0.25545899999999999</v>
       </c>
       <c r="Q36" t="s">
         <v>132</v>
@@ -17084,35 +17084,35 @@
         <v>36</v>
       </c>
       <c r="D37" s="19">
-        <v>-3.1049099999999998</v>
+        <v>-9.3295689999999993</v>
       </c>
       <c r="E37" s="19">
-        <v>3.6546690000000002</v>
+        <v>7.270251</v>
       </c>
       <c r="F37" s="19">
-        <v>30.485908999999999</v>
+        <v>41.514415999999997</v>
       </c>
       <c r="H37" t="s">
         <v>131</v>
       </c>
       <c r="I37" s="19">
-        <v>-1.0475650000000001</v>
+        <v>-0.97069899999999998</v>
       </c>
       <c r="J37" s="19">
-        <v>-0.146453</v>
+        <v>-0.21205099999999999</v>
       </c>
       <c r="K37" s="19">
-        <v>1E-4</v>
+        <v>-4.4771999999999999E-2</v>
       </c>
       <c r="L37" s="19"/>
       <c r="M37" s="19">
-        <v>-4.5045279999999996</v>
+        <v>-4.1740079999999997</v>
       </c>
       <c r="N37" s="19">
-        <v>-2.797641</v>
+        <v>-2.8766630000000002</v>
       </c>
       <c r="O37" s="19">
-        <v>-1.8016620000000001</v>
+        <v>-1.685686</v>
       </c>
       <c r="Q37" t="s">
         <v>132</v>
@@ -17135,35 +17135,35 @@
         <v>37</v>
       </c>
       <c r="D38" s="19">
-        <v>-5.4326749999999997</v>
+        <v>-10.269332</v>
       </c>
       <c r="E38" s="19">
-        <v>4.4149339999999997</v>
+        <v>10.340363</v>
       </c>
       <c r="F38" s="19">
-        <v>-4.0373700000000001</v>
+        <v>0.65954699999999999</v>
       </c>
       <c r="H38" t="s">
         <v>132</v>
       </c>
       <c r="I38" s="19">
-        <v>-1.225956</v>
+        <v>0.25024999999999997</v>
       </c>
       <c r="J38" s="19">
-        <v>-9.3627109999999991</v>
+        <v>-9.7925979999999999</v>
       </c>
       <c r="K38" s="19">
-        <v>6.6610060000000004</v>
+        <v>6.0079229999999999</v>
       </c>
       <c r="L38" s="19"/>
       <c r="M38" s="19">
-        <v>-5.2716089999999998</v>
+        <v>1.076076</v>
       </c>
       <c r="N38" s="19">
-        <v>-37.501690000000004</v>
+        <v>-35.928708</v>
       </c>
       <c r="O38" s="19">
-        <v>23.913433999999999</v>
+        <v>25.669978</v>
       </c>
       <c r="Q38" t="s">
         <v>132</v>
@@ -17186,35 +17186,35 @@
         <v>38</v>
       </c>
       <c r="D39" s="19">
-        <v>2.1852710000000002</v>
+        <v>-25.088291999999999</v>
       </c>
       <c r="E39" s="19">
-        <v>5.5832449999999998</v>
+        <v>25.084900999999999</v>
       </c>
       <c r="F39" s="19">
-        <v>26.211829000000002</v>
+        <v>79.869304</v>
       </c>
       <c r="H39" t="s">
         <v>132</v>
       </c>
       <c r="I39" s="19">
-        <v>14.013825000000001</v>
+        <v>11.443484</v>
       </c>
       <c r="J39" s="19">
-        <v>14.138628000000001</v>
+        <v>17.812508999999999</v>
       </c>
       <c r="K39" s="19">
-        <v>7.7808250000000001</v>
+        <v>10.455862</v>
       </c>
       <c r="L39" s="19"/>
       <c r="M39" s="19">
-        <v>60.259447000000002</v>
+        <v>49.206980999999999</v>
       </c>
       <c r="N39" s="19">
-        <v>82.780690000000007</v>
+        <v>90.935658000000004</v>
       </c>
       <c r="O39" s="19">
-        <v>28.138500000000001</v>
+        <v>25.281296000000001</v>
       </c>
       <c r="Q39" t="s">
         <v>132</v>
@@ -17237,23 +17237,23 @@
         <v>132</v>
       </c>
       <c r="I40" s="19">
-        <v>-7.6678600000000001</v>
+        <v>-33.006504</v>
       </c>
       <c r="J40" s="19">
-        <v>-16.385034999999998</v>
+        <v>49.226441000000001</v>
       </c>
       <c r="K40" s="19">
-        <v>5.7645</v>
+        <v>-370.03682500000002</v>
       </c>
       <c r="L40" s="19"/>
       <c r="M40" s="19">
-        <v>-32.971795999999998</v>
+        <v>-141.927966</v>
       </c>
       <c r="N40" s="19">
-        <v>-77.502280999999996</v>
+        <v>112.350815</v>
       </c>
       <c r="O40" s="19">
-        <v>17.796315</v>
+        <v>-976.90208299999995</v>
       </c>
       <c r="Q40" t="s">
         <v>132</v>
@@ -17282,23 +17282,23 @@
         <v>132</v>
       </c>
       <c r="I41" s="19">
-        <v>-7.9977479999999996</v>
+        <v>-6.5231209999999997</v>
       </c>
       <c r="J41" s="19">
-        <v>-1.0617760000000001</v>
+        <v>1.441972</v>
       </c>
       <c r="K41" s="19">
-        <v>9.7576920000000005</v>
+        <v>9.7396270000000005</v>
       </c>
       <c r="L41" s="19"/>
       <c r="M41" s="19">
-        <v>-34.390313999999996</v>
+        <v>-28.049420000000001</v>
       </c>
       <c r="N41" s="19">
-        <v>-21.149114999999998</v>
+        <v>-8.6549359999999993</v>
       </c>
       <c r="O41" s="19">
-        <v>8.8084380000000007</v>
+        <v>8.6597930000000005</v>
       </c>
       <c r="Q41" t="s">
         <v>132</v>
@@ -17329,35 +17329,35 @@
     </row>
     <row r="44" spans="3:21" x14ac:dyDescent="0.2">
       <c r="D44">
-        <v>51.847763999999998</v>
+        <v>53.598886999999998</v>
       </c>
       <c r="E44">
-        <v>-21.462334999999999</v>
+        <v>-20.685796</v>
       </c>
       <c r="F44">
-        <v>70.702804999999998</v>
+        <v>96.280077000000006</v>
       </c>
     </row>
     <row r="45" spans="3:21" x14ac:dyDescent="0.2">
       <c r="D45">
-        <v>-21.462334999999999</v>
+        <v>-20.685796</v>
       </c>
       <c r="E45">
-        <v>21.085536999999999</v>
+        <v>37.747810999999999</v>
       </c>
       <c r="F45">
-        <v>-9.3634529999999998</v>
+        <v>1.5296190000000001</v>
       </c>
     </row>
     <row r="46" spans="3:21" x14ac:dyDescent="0.2">
       <c r="D46">
-        <v>70.702804999999998</v>
+        <v>96.280077000000006</v>
       </c>
       <c r="E46">
-        <v>-9.3634529999999998</v>
+        <v>1.5296190000000001</v>
       </c>
       <c r="F46">
-        <v>60.790374999999997</v>
+        <v>185.23258999999999</v>
       </c>
     </row>
     <row r="47" spans="3:21" x14ac:dyDescent="0.2">
@@ -17388,9 +17388,6 @@
       <c r="M48" t="s">
         <v>207</v>
       </c>
-      <c r="Q48" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="49" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
@@ -17410,44 +17407,32 @@
       </c>
       <c r="I49">
         <f>(I5-I27)/I5</f>
-        <v>-1.0001328785499828</v>
+        <v>0</v>
       </c>
       <c r="J49">
         <f t="shared" ref="J49:K49" si="0">(J5-J27)/J5</f>
-        <v>-6.3995678354425808E-2</v>
+        <v>0</v>
       </c>
       <c r="K49">
         <f t="shared" si="0"/>
-        <v>-8.9601322109866734E-3</v>
+        <v>0</v>
       </c>
       <c r="L49" s="19"/>
       <c r="M49" s="65">
         <f>(M5-M27)/M5</f>
-        <v>-1.0001326967524742</v>
+        <v>0</v>
       </c>
       <c r="N49" s="65">
         <f t="shared" ref="N49:O49" si="1">(N5-N27)/N5</f>
-        <v>8.7096853218763731E-2</v>
+        <v>0</v>
       </c>
       <c r="O49" s="65">
         <f t="shared" si="1"/>
-        <v>-7.5068603536232209E-2</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>131</v>
-      </c>
-      <c r="R49" t="s">
-        <v>133</v>
-      </c>
-      <c r="S49" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="T49" s="7">
-        <v>0</v>
-      </c>
-      <c r="U49" s="7">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S49" s="7"/>
+      <c r="T49" s="7"/>
+      <c r="U49" s="7"/>
     </row>
     <row r="50" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
@@ -17467,44 +17452,32 @@
       </c>
       <c r="I50" s="65">
         <f t="shared" ref="I50:K50" si="2">(I6-I28)/I6</f>
-        <v>-0.15994006162204025</v>
+        <v>0</v>
       </c>
       <c r="J50" s="65">
         <f t="shared" si="2"/>
-        <v>-8.2129194368779995E-2</v>
+        <v>0</v>
       </c>
       <c r="K50" s="65">
         <f t="shared" si="2"/>
-        <v>-0.15162026334115275</v>
+        <v>0</v>
       </c>
       <c r="L50" s="19"/>
       <c r="M50" s="65">
         <f t="shared" ref="M50:O50" si="3">(M6-M28)/M6</f>
-        <v>-0.15994000704598985</v>
+        <v>0</v>
       </c>
       <c r="N50" s="65">
         <f t="shared" si="3"/>
-        <v>-0.12343768999365223</v>
+        <v>0</v>
       </c>
       <c r="O50" s="65">
         <f t="shared" si="3"/>
-        <v>-1.56197978293688</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>131</v>
-      </c>
-      <c r="R50" t="s">
-        <v>142</v>
-      </c>
-      <c r="S50" s="7">
-        <v>0.05</v>
-      </c>
-      <c r="T50" s="7">
-        <v>0</v>
-      </c>
-      <c r="U50" s="7">
-        <v>-0.15</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S50" s="7"/>
+      <c r="T50" s="7"/>
+      <c r="U50" s="7"/>
     </row>
     <row r="51" spans="3:21" x14ac:dyDescent="0.2">
       <c r="D51" s="19"/>
@@ -17515,44 +17488,32 @@
       </c>
       <c r="I51" s="65">
         <f t="shared" ref="I51:K51" si="4">(I7-I29)/I7</f>
-        <v>-7.9185283921845637E-2</v>
+        <v>0</v>
       </c>
       <c r="J51" s="65">
         <f t="shared" si="4"/>
-        <v>0.30935115713777439</v>
+        <v>0</v>
       </c>
       <c r="K51" s="65">
         <f t="shared" si="4"/>
-        <v>1.0022310460354882</v>
+        <v>0</v>
       </c>
       <c r="L51" s="19"/>
       <c r="M51" s="65">
         <f t="shared" ref="M51:O51" si="5">(M7-M29)/M7</f>
-        <v>-7.9185288191852055E-2</v>
+        <v>0</v>
       </c>
       <c r="N51" s="65">
         <f t="shared" si="5"/>
-        <v>2.7469989045561867E-2</v>
+        <v>0</v>
       </c>
       <c r="O51" s="65">
         <f t="shared" si="5"/>
-        <v>-6.8800269669272662E-2</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>131</v>
-      </c>
-      <c r="R51" t="s">
-        <v>133</v>
-      </c>
-      <c r="S51" s="7">
-        <v>0.49</v>
-      </c>
-      <c r="T51" s="7">
-        <v>0.52</v>
-      </c>
-      <c r="U51" s="7">
-        <v>2.5000000000000001E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S51" s="7"/>
+      <c r="T51" s="7"/>
+      <c r="U51" s="7"/>
     </row>
     <row r="52" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
@@ -17566,44 +17527,32 @@
       </c>
       <c r="I52" s="65">
         <f t="shared" ref="I52:K52" si="6">(I8-I30)/I8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J52" s="65">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52" s="65">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52" s="19"/>
       <c r="M52" s="65">
         <f t="shared" ref="M52:O52" si="7">(M8-M30)/M8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N52" s="65">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O52" s="65">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>131</v>
-      </c>
-      <c r="R52" t="s">
-        <v>142</v>
-      </c>
-      <c r="S52" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="T52" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="U52" s="7">
-        <v>2.5000000000000001E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S52" s="7"/>
+      <c r="T52" s="7"/>
+      <c r="U52" s="7"/>
     </row>
     <row r="53" spans="3:21" x14ac:dyDescent="0.2">
       <c r="D53" s="19" t="s">
@@ -17620,44 +17569,32 @@
       </c>
       <c r="I53" s="65">
         <f t="shared" ref="I53:K53" si="8">(I9-I31)/I9</f>
-        <v>5.8989054988791256</v>
+        <v>0</v>
       </c>
       <c r="J53" s="65">
         <f t="shared" si="8"/>
-        <v>4.3898977972850362E-2</v>
+        <v>0</v>
       </c>
       <c r="K53" s="65">
         <f t="shared" si="8"/>
-        <v>-0.10870345708491927</v>
+        <v>0</v>
       </c>
       <c r="L53" s="19"/>
       <c r="M53" s="65">
         <f t="shared" ref="M53:O53" si="9">(M9-M31)/M9</f>
-        <v>5.8989188495979841</v>
+        <v>0</v>
       </c>
       <c r="N53" s="65">
         <f t="shared" si="9"/>
-        <v>-4.3780616881631221E-2</v>
+        <v>0</v>
       </c>
       <c r="O53" s="65">
         <f t="shared" si="9"/>
-        <v>6.8427875880060177E-2</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>131</v>
-      </c>
-      <c r="R53" t="s">
-        <v>133</v>
-      </c>
-      <c r="S53" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="T53" s="7">
-        <v>0</v>
-      </c>
-      <c r="U53" s="7">
-        <v>0.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S53" s="7"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
     </row>
     <row r="54" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
@@ -17677,44 +17614,32 @@
       </c>
       <c r="I54" s="65">
         <f t="shared" ref="I54:K54" si="10">(I10-I32)/I10</f>
-        <v>-0.21599452999620081</v>
+        <v>0</v>
       </c>
       <c r="J54" s="65">
         <f t="shared" si="10"/>
-        <v>0.24568028352474844</v>
+        <v>0</v>
       </c>
       <c r="K54" s="65">
         <f t="shared" si="10"/>
-        <v>0.20493412138924794</v>
+        <v>0</v>
       </c>
       <c r="L54" s="19"/>
       <c r="M54" s="65">
         <f t="shared" ref="M54:O54" si="11">(M10-M32)/M10</f>
-        <v>-0.21599461438334952</v>
+        <v>0</v>
       </c>
       <c r="N54" s="65">
         <f t="shared" si="11"/>
-        <v>9.9356994708792071E-2</v>
+        <v>0</v>
       </c>
       <c r="O54" s="65">
         <f t="shared" si="11"/>
-        <v>-0.13262446680945669</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>131</v>
-      </c>
-      <c r="R54" t="s">
-        <v>142</v>
-      </c>
-      <c r="S54" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="T54" s="7">
-        <v>0</v>
-      </c>
-      <c r="U54" s="7">
-        <v>0.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S54" s="7"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="7"/>
     </row>
     <row r="55" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
@@ -17734,44 +17659,32 @@
       </c>
       <c r="I55" s="65">
         <f t="shared" ref="I55:K55" si="12">(I11-I33)/I11</f>
-        <v>1.2340122180433444</v>
+        <v>0</v>
       </c>
       <c r="J55" s="65">
         <f t="shared" si="12"/>
-        <v>1.1075465603398797</v>
+        <v>0</v>
       </c>
       <c r="K55" s="65">
         <f t="shared" si="12"/>
-        <v>1.0269659006839322</v>
+        <v>0</v>
       </c>
       <c r="L55" s="19"/>
       <c r="M55" s="65">
         <f t="shared" ref="M55:O55" si="13">(M11-M33)/M11</f>
-        <v>1.234012189183316</v>
+        <v>0</v>
       </c>
       <c r="N55" s="65">
         <f t="shared" si="13"/>
-        <v>1.1279470661210023</v>
+        <v>0</v>
       </c>
       <c r="O55" s="65">
         <f t="shared" si="13"/>
-        <v>1.0225506987474342</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>205</v>
-      </c>
-      <c r="R55" t="s">
-        <v>209</v>
-      </c>
-      <c r="S55" s="7">
-        <v>0</v>
-      </c>
-      <c r="T55" s="7">
-        <v>0.52</v>
-      </c>
-      <c r="U55" s="7">
-        <v>0.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="7"/>
     </row>
     <row r="56" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
@@ -17791,44 +17704,32 @@
       </c>
       <c r="I56" s="65">
         <f t="shared" ref="I56:K56" si="14">(I12-I34)/I12</f>
-        <v>-0.22606138594372469</v>
+        <v>0</v>
       </c>
       <c r="J56" s="65">
         <f t="shared" si="14"/>
-        <v>1.7363358902502199</v>
+        <v>0</v>
       </c>
       <c r="K56" s="65">
         <f t="shared" si="14"/>
-        <v>-1.8548966869981027E-3</v>
+        <v>0</v>
       </c>
       <c r="L56" s="19"/>
       <c r="M56" s="65">
         <f t="shared" ref="M56:O56" si="15">(M12-M34)/M12</f>
-        <v>-0.22606145773918113</v>
+        <v>0</v>
       </c>
       <c r="N56" s="65">
         <f t="shared" si="15"/>
-        <v>-1.443589710705</v>
+        <v>0</v>
       </c>
       <c r="O56" s="65">
         <f t="shared" si="15"/>
-        <v>-1.7164842489324698E-2</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>132</v>
-      </c>
-      <c r="R56" t="s">
-        <v>133</v>
-      </c>
-      <c r="S56" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="T56" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="U56" s="7">
-        <v>0.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
     </row>
     <row r="57" spans="3:21" x14ac:dyDescent="0.2">
       <c r="D57" s="19"/>
@@ -17839,44 +17740,32 @@
       </c>
       <c r="I57" s="65">
         <f t="shared" ref="I57:K57" si="16">(I13-I35)/I13</f>
-        <v>-3.9667258424486367E-2</v>
+        <v>0</v>
       </c>
       <c r="J57" s="65">
         <f t="shared" si="16"/>
-        <v>0.22687912709369443</v>
+        <v>0</v>
       </c>
       <c r="K57" s="65">
         <f t="shared" si="16"/>
-        <v>-0.23586330331674035</v>
+        <v>0</v>
       </c>
       <c r="L57" s="19"/>
       <c r="M57" s="65">
         <f t="shared" ref="M57:O57" si="17">(M13-M35)/M13</f>
-        <v>-3.9667532141231449E-2</v>
+        <v>0</v>
       </c>
       <c r="N57" s="65">
         <f t="shared" si="17"/>
-        <v>1.5730231103912206E-2</v>
+        <v>0</v>
       </c>
       <c r="O57" s="65">
         <f t="shared" si="17"/>
-        <v>-0.10768570232576251</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>132</v>
-      </c>
-      <c r="R57" t="s">
-        <v>142</v>
-      </c>
-      <c r="S57" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="T57" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="U57" s="7">
-        <v>0.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
     </row>
     <row r="58" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C58" s="26" t="s">
@@ -17896,44 +17785,32 @@
       </c>
       <c r="I58" s="65">
         <f t="shared" ref="I58:K58" si="18">(I14-I36)/I14</f>
-        <v>-0.24654168249978087</v>
+        <v>0</v>
       </c>
       <c r="J58" s="65">
         <f t="shared" si="18"/>
-        <v>1.175611438046496E-2</v>
+        <v>0</v>
       </c>
       <c r="K58" s="65">
         <f t="shared" si="18"/>
-        <v>-0.34277481912605373</v>
+        <v>0</v>
       </c>
       <c r="L58" s="19"/>
       <c r="M58" s="65">
         <f t="shared" ref="M58:O58" si="19">(M14-M36)/M14</f>
-        <v>-0.24654163883833058</v>
+        <v>0</v>
       </c>
       <c r="N58" s="65">
         <f t="shared" si="19"/>
-        <v>-0.13041862627459777</v>
+        <v>0</v>
       </c>
       <c r="O58" s="65">
         <f t="shared" si="19"/>
-        <v>-0.39131132588791157</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>132</v>
-      </c>
-      <c r="R58" t="s">
-        <v>133</v>
-      </c>
-      <c r="S58" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="T58" s="7">
-        <v>0</v>
-      </c>
-      <c r="U58" s="7">
-        <v>-0.04</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S58" s="7"/>
+      <c r="T58" s="7"/>
+      <c r="U58" s="7"/>
     </row>
     <row r="59" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
@@ -17941,59 +17818,47 @@
       </c>
       <c r="D59" s="65">
         <f>(D15-D37)/D15</f>
-        <v>0.66719684478457686</v>
+        <v>0</v>
       </c>
       <c r="E59" s="65">
         <f t="shared" ref="E59:F59" si="20">(E15-E37)/E15</f>
-        <v>0.49731185346970824</v>
+        <v>0</v>
       </c>
       <c r="F59" s="65">
         <f t="shared" si="20"/>
-        <v>0.2656548751643284</v>
+        <v>0</v>
       </c>
       <c r="H59" t="s">
         <v>131</v>
       </c>
       <c r="I59" s="65">
         <f t="shared" ref="I59:K59" si="21">(I15-I37)/I15</f>
-        <v>-7.9186235898048837E-2</v>
+        <v>0</v>
       </c>
       <c r="J59" s="65">
         <f t="shared" si="21"/>
-        <v>0.30935010917185013</v>
+        <v>0</v>
       </c>
       <c r="K59" s="65">
         <f t="shared" si="21"/>
-        <v>1.0022335388189048</v>
+        <v>0</v>
       </c>
       <c r="L59" s="19"/>
       <c r="M59" s="65">
         <f t="shared" ref="M59:O59" si="22">(M15-M37)/M15</f>
-        <v>-7.9185281868170823E-2</v>
+        <v>0</v>
       </c>
       <c r="N59" s="65">
         <f t="shared" si="22"/>
-        <v>2.7470023426449375E-2</v>
+        <v>0</v>
       </c>
       <c r="O59" s="65">
         <f t="shared" si="22"/>
-        <v>-6.8800476482571538E-2</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>132</v>
-      </c>
-      <c r="R59" t="s">
-        <v>142</v>
-      </c>
-      <c r="S59" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="T59" s="7">
-        <v>0</v>
-      </c>
-      <c r="U59" s="7">
-        <v>-0.03</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S59" s="7"/>
+      <c r="T59" s="7"/>
+      <c r="U59" s="7"/>
     </row>
     <row r="60" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
@@ -18001,59 +17866,47 @@
       </c>
       <c r="D60" s="65">
         <f t="shared" ref="D60:F60" si="23">(D16-D38)/D16</f>
-        <v>0.47098068306682467</v>
+        <v>0</v>
       </c>
       <c r="E60" s="65">
         <f t="shared" si="23"/>
-        <v>0.57303878016661502</v>
+        <v>0</v>
       </c>
       <c r="F60" s="65">
         <f t="shared" si="23"/>
-        <v>7.1214287988573979</v>
+        <v>0</v>
       </c>
       <c r="H60" t="s">
         <v>132</v>
       </c>
       <c r="I60" s="65">
         <f t="shared" ref="I60:K60" si="24">(I16-I38)/I16</f>
-        <v>5.8989250749250752</v>
+        <v>0</v>
       </c>
       <c r="J60" s="65">
         <f t="shared" si="24"/>
-        <v>4.3899177725870174E-2</v>
+        <v>0</v>
       </c>
       <c r="K60" s="65">
         <f t="shared" si="24"/>
-        <v>-0.10870362353179303</v>
+        <v>0</v>
       </c>
       <c r="L60" s="19"/>
       <c r="M60" s="65">
         <f t="shared" ref="M60:O60" si="25">(M16-M38)/M16</f>
-        <v>5.8989188495979841</v>
+        <v>0</v>
       </c>
       <c r="N60" s="65">
         <f t="shared" si="25"/>
-        <v>-4.3780644714527535E-2</v>
+        <v>0</v>
       </c>
       <c r="O60" s="65">
         <f t="shared" si="25"/>
-        <v>6.8427951126409287E-2</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>132</v>
-      </c>
-      <c r="R60" t="s">
-        <v>133</v>
-      </c>
-      <c r="S60" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="T60" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="U60" s="7">
-        <v>0.32</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S60" s="7"/>
+      <c r="T60" s="7"/>
+      <c r="U60" s="7"/>
     </row>
     <row r="61" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
@@ -18061,59 +17914,47 @@
       </c>
       <c r="D61" s="65">
         <f t="shared" ref="D61:F61" si="26">(D17-D39)/D17</f>
-        <v>1.0871032193024539</v>
+        <v>0</v>
       </c>
       <c r="E61" s="65">
         <f t="shared" si="26"/>
-        <v>0.77742606996934127</v>
+        <v>0</v>
       </c>
       <c r="F61" s="65">
         <f t="shared" si="26"/>
-        <v>0.6718159832718712</v>
+        <v>0</v>
       </c>
       <c r="H61" t="s">
         <v>132</v>
       </c>
       <c r="I61" s="65">
         <f t="shared" ref="I61:K61" si="27">(I17-I39)/I17</f>
-        <v>-0.22461175285428817</v>
+        <v>0</v>
       </c>
       <c r="J61" s="65">
         <f t="shared" si="27"/>
-        <v>0.20625286420907904</v>
+        <v>0</v>
       </c>
       <c r="K61" s="65">
         <f t="shared" si="27"/>
-        <v>0.25584088619379253</v>
+        <v>0</v>
       </c>
       <c r="L61" s="19"/>
       <c r="M61" s="65">
         <f t="shared" ref="M61:O61" si="28">(M17-M39)/M17</f>
-        <v>-0.22461174767051859</v>
+        <v>0</v>
       </c>
       <c r="N61" s="65">
         <f t="shared" si="28"/>
-        <v>8.9678440551889962E-2</v>
+        <v>0</v>
       </c>
       <c r="O61" s="65">
         <f t="shared" si="28"/>
-        <v>-0.11301651624188884</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>132</v>
-      </c>
-      <c r="R61" t="s">
-        <v>142</v>
-      </c>
-      <c r="S61" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="T61" s="7">
-        <v>0.48</v>
-      </c>
-      <c r="U61" s="7">
-        <v>0.3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S61" s="7"/>
+      <c r="T61" s="7"/>
+      <c r="U61" s="7"/>
     </row>
     <row r="62" spans="3:21" x14ac:dyDescent="0.2">
       <c r="H62" t="s">
@@ -18121,44 +17962,32 @@
       </c>
       <c r="I62" s="65">
         <f t="shared" ref="I62:K62" si="29">(I18-I40)/I18</f>
-        <v>0.76768639296061159</v>
+        <v>0</v>
       </c>
       <c r="J62" s="65">
         <f t="shared" si="29"/>
-        <v>1.332850286698565</v>
+        <v>0</v>
       </c>
       <c r="K62" s="65">
         <f t="shared" si="29"/>
-        <v>1.0155781792798595</v>
+        <v>0</v>
       </c>
       <c r="L62" s="19"/>
       <c r="M62" s="65">
         <f t="shared" ref="M62:O62" si="30">(M18-M40)/M18</f>
-        <v>0.76768640508805719</v>
+        <v>0</v>
       </c>
       <c r="N62" s="65">
         <f t="shared" si="30"/>
-        <v>1.6898239322963522</v>
+        <v>0</v>
       </c>
       <c r="O62" s="65">
         <f t="shared" si="30"/>
-        <v>1.0182170918761364</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>132</v>
-      </c>
-      <c r="R62" t="s">
-        <v>133</v>
-      </c>
-      <c r="S62" s="7">
-        <v>0</v>
-      </c>
-      <c r="T62" s="7">
-        <v>0</v>
-      </c>
-      <c r="U62" s="7">
-        <v>0.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S62" s="7"/>
+      <c r="T62" s="7"/>
+      <c r="U62" s="7"/>
     </row>
     <row r="63" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C63" s="26" t="s">
@@ -18172,44 +18001,32 @@
       </c>
       <c r="I63" s="65">
         <f t="shared" ref="I63:K63" si="31">(I19-I41)/I19</f>
-        <v>-0.22606157389997825</v>
+        <v>0</v>
       </c>
       <c r="J63" s="65">
         <f t="shared" si="31"/>
-        <v>1.7363360730998936</v>
+        <v>0</v>
       </c>
       <c r="K63" s="65">
         <f t="shared" si="31"/>
-        <v>-1.8547938232131474E-3</v>
+        <v>0</v>
       </c>
       <c r="L63" s="19"/>
       <c r="M63" s="65">
         <f t="shared" ref="M63:O63" si="32">(M19-M41)/M19</f>
-        <v>-0.22606150144994067</v>
+        <v>0</v>
       </c>
       <c r="N63" s="65">
         <f t="shared" si="32"/>
-        <v>-1.4435899930398099</v>
+        <v>0</v>
       </c>
       <c r="O63" s="65">
         <f t="shared" si="32"/>
-        <v>-1.7164959947656964E-2</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>132</v>
-      </c>
-      <c r="R63" t="s">
-        <v>142</v>
-      </c>
-      <c r="S63" s="7">
-        <v>0</v>
-      </c>
-      <c r="T63" s="7">
-        <v>0</v>
-      </c>
-      <c r="U63" s="7">
-        <v>0.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S63" s="7"/>
+      <c r="T63" s="7"/>
+      <c r="U63" s="7"/>
     </row>
     <row r="64" spans="3:21" x14ac:dyDescent="0.2">
       <c r="T64" s="7"/>
@@ -18225,43 +18042,43 @@
     <row r="66" spans="3:21" x14ac:dyDescent="0.2">
       <c r="D66" s="65">
         <f>(D22-D44)/D22</f>
-        <v>3.2670883632341094E-2</v>
+        <v>0</v>
       </c>
       <c r="E66" s="65">
         <f t="shared" ref="E66:F66" si="33">(E22-E44)/E22</f>
-        <v>-3.7539720492264339E-2</v>
+        <v>0</v>
       </c>
       <c r="F66" s="65">
         <f t="shared" si="33"/>
-        <v>0.26565487686512762</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="3:21" x14ac:dyDescent="0.2">
       <c r="D67" s="65">
         <f t="shared" ref="D67:F67" si="34">(D23-D45)/D23</f>
-        <v>-3.7539720492264339E-2</v>
+        <v>0</v>
       </c>
       <c r="E67" s="65">
         <f t="shared" si="34"/>
-        <v>0.44141033767494492</v>
+        <v>0</v>
       </c>
       <c r="F67" s="65">
         <f t="shared" si="34"/>
-        <v>7.1214282772376647</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="3:21" x14ac:dyDescent="0.2">
       <c r="D68" s="65">
         <f t="shared" ref="D68:F68" si="35">(D24-D46)/D24</f>
-        <v>0.26565487686512762</v>
+        <v>0</v>
       </c>
       <c r="E68" s="65">
         <f t="shared" si="35"/>
-        <v>7.1214282772376647</v>
+        <v>0</v>
       </c>
       <c r="F68" s="65">
         <f t="shared" si="35"/>
-        <v>0.67181598551313237</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LonePair H Matrix Integral - 1
</commit_message>
<xml_diff>
--- a/SLAM_Ext/validation/EwaldTestValidation.xlsx
+++ b/SLAM_Ext/validation/EwaldTestValidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/woongkyujee/Desktop/ProjectPAX/SLAM Extension Reference/SLAM-3D-Extension/SLAM_Ext/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B039DB1-E819-B042-8070-68F6103F04CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6DBC9A-A387-E744-AC82-6203F36441AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17100" yWindow="1000" windowWidth="47980" windowHeight="25400" firstSheet="4" activeTab="16" xr2:uid="{ED569559-3BE8-BA43-B08A-1C36884B8A7F}"/>
   </bookViews>
@@ -15779,7 +15779,7 @@
   <dimension ref="C4:V68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>